<commit_message>
feat: expand global multi-asset fixtures with matched scenarios
</commit_message>
<xml_diff>
--- a/examples/integration-harness/src/main/resources/data/global-multi-asset/apac_positions.xlsx
+++ b/examples/integration-harness/src/main/resources/data/global-multi-asset/apac_positions.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -769,6 +769,228 @@
       </c>
       <c r="Y3" t="n">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TRD-DEMO1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>L-DEMO</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ALLOC-DEMO1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>DEMO-PORT</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ISIN-DEMO1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2024/08/25</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024/08/27</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0092</v>
+      </c>
+      <c r="J4" t="n">
+        <v>100000</v>
+      </c>
+      <c r="K4" t="n">
+        <v>99500</v>
+      </c>
+      <c r="L4" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="M4" t="n">
+        <v>175</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="O4" t="n">
+        <v>166.4</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>READY</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>AFFIRMED</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>DemoCounterparty</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>DemoBroker</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>GLOBAL</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>GLOBAL-DEMO</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Tokyo</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>MATCH-CONFIRMED</t>
+        </is>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TRD-DEMO2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>L-DEMO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ALLOC-DEMO2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>DEMO-PORT</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ISIN-DEMO2</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>JPY</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2024/08/21</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024/08/23</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0092</v>
+      </c>
+      <c r="J5" t="n">
+        <v>255000</v>
+      </c>
+      <c r="K5" t="n">
+        <v>254600</v>
+      </c>
+      <c r="L5" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="M5" t="n">
+        <v>175</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="O5" t="n">
+        <v>169.4</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>READY</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>AFFIRMED</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>APAC-PRIME</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>BRK-TKY</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>APAC</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>APAC-DEMO</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Tokyo</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>Synthetic mismatch</t>
+        </is>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>